<commit_message>
Minor Fix: a cell's boarder was missing
</commit_message>
<xml_diff>
--- a/BOMs/BOM#1.xlsx
+++ b/BOMs/BOM#1.xlsx
@@ -419,6 +419,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
@@ -770,6 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5486,6 +5490,9 @@
       <c r="B998" s="16"/>
     </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>